<commit_message>
Update tablas pedidos especiales
Update tablas pedidos especiales
</commit_message>
<xml_diff>
--- a/Analisis/SPRINTs/Tablas pedidos especiales.xlsx
+++ b/Analisis/SPRINTs/Tablas pedidos especiales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents\comercializadora\Analisis\SPRINTs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8339C95-7C44-4A7C-8021-7D616FB2D727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD22EE20-5A8B-4B98-85E9-41AC0C9455CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{A9D406EB-54B5-4C49-A6DD-DF39C8714232}"/>
   </bookViews>
@@ -736,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA8782D-A63D-4DA9-826A-39AC8BB65894}">
   <dimension ref="A2:K56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>